<commit_message>
add median to the stats
</commit_message>
<xml_diff>
--- a/02-output/Raters_names.xlsx
+++ b/02-output/Raters_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Rater</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
   </si>
   <si>
     <t>std</t>
@@ -467,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,10 +504,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>4623</v>
@@ -513,27 +519,30 @@
         <v>91.10728963876271</v>
       </c>
       <c r="D2">
+        <v>91</v>
+      </c>
+      <c r="E2">
         <v>2.528709422063331</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>80</v>
       </c>
-      <c r="F2">
-        <v>89</v>
-      </c>
       <c r="G2">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H2">
+        <v>91</v>
+      </c>
+      <c r="I2">
         <v>93</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>127</v>
@@ -542,27 +551,30 @@
         <v>90.86614173228347</v>
       </c>
       <c r="D3">
+        <v>91</v>
+      </c>
+      <c r="E3">
         <v>1.692008315134027</v>
       </c>
-      <c r="E3">
-        <v>87</v>
-      </c>
       <c r="F3">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G3">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3">
+        <v>91</v>
+      </c>
+      <c r="I3">
         <v>92</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>11589</v>
@@ -571,27 +583,30 @@
         <v>90.52282336698593</v>
       </c>
       <c r="D4">
+        <v>91</v>
+      </c>
+      <c r="E4">
         <v>2.523811579633453</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>81</v>
       </c>
-      <c r="F4">
-        <v>89</v>
-      </c>
       <c r="G4">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H4">
+        <v>91</v>
+      </c>
+      <c r="I4">
         <v>92</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1356</v>
@@ -600,27 +615,30 @@
         <v>90.0117994100295</v>
       </c>
       <c r="D5">
+        <v>90</v>
+      </c>
+      <c r="E5">
         <v>3.091448890589783</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>82</v>
       </c>
-      <c r="F5">
-        <v>88</v>
-      </c>
       <c r="G5">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H5">
+        <v>90</v>
+      </c>
+      <c r="I5">
         <v>92</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>1292</v>
@@ -629,27 +647,30 @@
         <v>89.85758513931889</v>
       </c>
       <c r="D6">
+        <v>90</v>
+      </c>
+      <c r="E6">
         <v>2.4986124213751</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>82</v>
       </c>
-      <c r="F6">
-        <v>88</v>
-      </c>
       <c r="G6">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I6">
+        <v>91</v>
+      </c>
+      <c r="J6">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>13198</v>
@@ -658,27 +679,30 @@
         <v>89.79481739657524</v>
       </c>
       <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7">
         <v>3.148810628454373</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>80</v>
       </c>
-      <c r="F7">
-        <v>88</v>
-      </c>
       <c r="G7">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7">
         <v>92</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>11494</v>
@@ -687,27 +711,30 @@
         <v>89.39081259787716</v>
       </c>
       <c r="D8">
+        <v>90</v>
+      </c>
+      <c r="E8">
         <v>2.819591714081941</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>80</v>
       </c>
-      <c r="F8">
-        <v>87</v>
-      </c>
       <c r="G8">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H8">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I8">
+        <v>91</v>
+      </c>
+      <c r="J8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>14057</v>
@@ -716,27 +743,30 @@
         <v>89.31856014796898</v>
       </c>
       <c r="D9">
+        <v>89</v>
+      </c>
+      <c r="E9">
         <v>2.660626502319701</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>80</v>
       </c>
-      <c r="F9">
-        <v>87</v>
-      </c>
       <c r="G9">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H9">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I9">
+        <v>91</v>
+      </c>
+      <c r="J9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>196</v>
@@ -745,27 +775,30 @@
         <v>89.26020408163265</v>
       </c>
       <c r="D10">
+        <v>89</v>
+      </c>
+      <c r="E10">
         <v>2.080100579221005</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>83</v>
       </c>
-      <c r="F10">
-        <v>88</v>
-      </c>
       <c r="G10">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H10">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I10">
+        <v>91</v>
+      </c>
+      <c r="J10">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>7328</v>
@@ -774,27 +807,30 @@
         <v>89.1112172489083</v>
       </c>
       <c r="D11">
+        <v>89</v>
+      </c>
+      <c r="E11">
         <v>2.443418892455772</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>80</v>
       </c>
-      <c r="F11">
-        <v>87</v>
-      </c>
       <c r="G11">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H11">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I11">
+        <v>91</v>
+      </c>
+      <c r="J11">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>7681</v>
@@ -803,27 +839,30 @@
         <v>89.00260382762661</v>
       </c>
       <c r="D12">
+        <v>89</v>
+      </c>
+      <c r="E12">
         <v>2.835322859781385</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>80</v>
       </c>
-      <c r="F12">
-        <v>87</v>
-      </c>
       <c r="G12">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H12">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I12">
+        <v>91</v>
+      </c>
+      <c r="J12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>29502</v>
@@ -832,27 +871,30 @@
         <v>88.87505931801233</v>
       </c>
       <c r="D13">
+        <v>89</v>
+      </c>
+      <c r="E13">
         <v>2.921718395041843</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>80</v>
       </c>
-      <c r="F13">
-        <v>87</v>
-      </c>
       <c r="G13">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H13">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I13">
+        <v>91</v>
+      </c>
+      <c r="J13">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>163</v>
@@ -861,27 +903,30 @@
         <v>88.61349693251533</v>
       </c>
       <c r="D14">
+        <v>88</v>
+      </c>
+      <c r="E14">
         <v>2.529639493600447</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>82</v>
       </c>
-      <c r="F14">
-        <v>87</v>
-      </c>
       <c r="G14">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I14">
+        <v>90</v>
+      </c>
+      <c r="J14">
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>5012</v>
@@ -890,27 +935,30 @@
         <v>88.53950518754988</v>
       </c>
       <c r="D15">
+        <v>89</v>
+      </c>
+      <c r="E15">
         <v>2.864852415043586</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>80</v>
       </c>
-      <c r="F15">
-        <v>87</v>
-      </c>
       <c r="G15">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H15">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I15">
+        <v>91</v>
+      </c>
+      <c r="J15">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>743</v>
@@ -919,27 +967,30 @@
         <v>88.4885598923284</v>
       </c>
       <c r="D16">
+        <v>89</v>
+      </c>
+      <c r="E16">
         <v>2.507039350717135</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>81</v>
       </c>
-      <c r="F16">
-        <v>87</v>
-      </c>
       <c r="G16">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H16">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I16">
+        <v>90</v>
+      </c>
+      <c r="J16">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>4369</v>
@@ -948,27 +999,30 @@
         <v>88.4051270313573</v>
       </c>
       <c r="D17">
+        <v>88</v>
+      </c>
+      <c r="E17">
         <v>2.561734347086102</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>80</v>
       </c>
-      <c r="F17">
-        <v>87</v>
-      </c>
       <c r="G17">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I17">
+        <v>90</v>
+      </c>
+      <c r="J17">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>21</v>
@@ -977,16 +1031,16 @@
         <v>88.14285714285714</v>
       </c>
       <c r="D18">
+        <v>89</v>
+      </c>
+      <c r="E18">
         <v>1.062342425290183</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>86</v>
       </c>
-      <c r="F18">
-        <v>87</v>
-      </c>
       <c r="G18">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H18">
         <v>89</v>
@@ -994,10 +1048,13 @@
       <c r="I18">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>1919</v>
@@ -1006,27 +1063,30 @@
         <v>87.7853048462741</v>
       </c>
       <c r="D19">
+        <v>88</v>
+      </c>
+      <c r="E19">
         <v>2.509371963672827</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>81</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>86</v>
       </c>
-      <c r="G19">
-        <v>88</v>
-      </c>
       <c r="H19">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I19">
+        <v>90</v>
+      </c>
+      <c r="J19">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>1551</v>
@@ -1035,27 +1095,30 @@
         <v>87.68407479045777</v>
       </c>
       <c r="D20">
+        <v>88</v>
+      </c>
+      <c r="E20">
         <v>2.598659287988316</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>80</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>86</v>
       </c>
-      <c r="G20">
-        <v>88</v>
-      </c>
       <c r="H20">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I20">
+        <v>90</v>
+      </c>
+      <c r="J20">
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>349</v>
@@ -1064,27 +1127,30 @@
         <v>87.40401146131805</v>
       </c>
       <c r="D21">
+        <v>88</v>
+      </c>
+      <c r="E21">
         <v>2.121343631867775</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>80</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>86</v>
       </c>
-      <c r="G21">
-        <v>88</v>
-      </c>
       <c r="H21">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I21">
+        <v>89</v>
+      </c>
+      <c r="J21">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>16200</v>
@@ -1093,27 +1159,30 @@
         <v>87.01117283950617</v>
       </c>
       <c r="D22">
+        <v>87</v>
+      </c>
+      <c r="E22">
         <v>3.051960432272369</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>80</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>85</v>
       </c>
-      <c r="G22">
-        <v>87</v>
-      </c>
       <c r="H22">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I22">
+        <v>89</v>
+      </c>
+      <c r="J22">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>1073</v>
@@ -1122,27 +1191,30 @@
         <v>86.62068965517241</v>
       </c>
       <c r="D23">
+        <v>87</v>
+      </c>
+      <c r="E23">
         <v>2.369075621429478</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>80</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>85</v>
       </c>
-      <c r="G23">
-        <v>87</v>
-      </c>
       <c r="H23">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I23">
+        <v>88</v>
+      </c>
+      <c r="J23">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>138</v>
@@ -1151,21 +1223,24 @@
         <v>86.3840579710145</v>
       </c>
       <c r="D24">
+        <v>87</v>
+      </c>
+      <c r="E24">
         <v>2.001176529010988</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>81</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>85</v>
       </c>
-      <c r="G24">
-        <v>87</v>
-      </c>
       <c r="H24">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I24">
+        <v>88</v>
+      </c>
+      <c r="J24">
         <v>92</v>
       </c>
     </row>

</xml_diff>